<commit_message>
Fixed minor issues in the report. Updated logs. Updated submission folder
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-0779-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-0779-350-1201.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\350FinalProject\ExU\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CE87BC-AAF0-420C-88B5-BE26840C1E7B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C789BA10-9A7C-47ED-A373-9C419A56ED78}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>Drew block diagram of Adder entity</t>
+  </si>
+  <si>
+    <t>Final verification of our code</t>
+  </si>
+  <si>
+    <t>Final check on report; redid Timing Logic Unit screenshots</t>
+  </si>
+  <si>
+    <t>Wrote and revised introduction of report</t>
   </si>
 </sst>
 </file>
@@ -417,14 +426,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
-  <dimension ref="A1:G758"/>
+  <dimension ref="A1:G759"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,21 +769,21 @@
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="28">
         <v>301290779</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -823,7 +832,7 @@
       <c r="E6" s="21">
         <v>0.7583333333333333</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="25" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1049,7 +1058,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="28">
+      <c r="B20" s="26">
         <v>779</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -1066,25 +1075,55 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="13"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="22"/>
-      <c r="G21" s="13"/>
+      <c r="B21" s="13">
+        <v>779</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="19">
+        <v>0.8354166666666667</v>
+      </c>
+      <c r="E21" s="22">
+        <v>0.85069444444444453</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="13"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="22"/>
-      <c r="G22" s="13"/>
+      <c r="B22" s="13">
+        <v>779</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="19">
+        <v>0.85069444444444453</v>
+      </c>
+      <c r="E22" s="22">
+        <v>0.92847222222222225</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="23" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="13"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="22"/>
-      <c r="G23" s="13"/>
+      <c r="B23" s="13">
+        <v>779</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="19">
+        <v>0.92847222222222225</v>
+      </c>
+      <c r="E23" s="22">
+        <v>0.97361111111111109</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="13"/>
@@ -1296,14 +1335,20 @@
       <c r="E53" s="22"/>
       <c r="G53" s="13"/>
     </row>
-    <row r="54" spans="2:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="14"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="23"/>
-      <c r="G54" s="14"/>
-    </row>
-    <row r="55" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="13"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="22"/>
+      <c r="G54" s="13"/>
+    </row>
+    <row r="55" spans="2:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="14"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="23"/>
+      <c r="G55" s="14"/>
+    </row>
     <row r="56" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2007,6 +2052,7 @@
     <row r="756" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="757" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="758" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>

</xml_diff>

<commit_message>
Fixed minor issues and updated doc
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-0779-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-0779-350-1201.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\ensc350-finalproject\ExU\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C789BA10-9A7C-47ED-A373-9C419A56ED78}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DF889A-6DB8-49CB-8C42-66DFEE1E2906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Wrote and revised introduction of report</t>
+  </si>
+  <si>
+    <t>Reviewed report together with team member for possible issues.</t>
+  </si>
+  <si>
+    <t>Revised report together with team member for clarity</t>
   </si>
 </sst>
 </file>
@@ -750,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G759"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,18 +1132,38 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="22"/>
-      <c r="G24" s="13"/>
+      <c r="B24" s="13">
+        <v>779</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="16">
+        <v>0.98402777777777783</v>
+      </c>
+      <c r="E24" s="22">
+        <v>0.99097222222222225</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="25" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="13"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="22"/>
-      <c r="G25" s="13"/>
+      <c r="B25" s="13">
+        <v>779</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="16">
+        <v>0.99097222222222225</v>
+      </c>
+      <c r="E25" s="22">
+        <v>0.99652777777777779</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="26" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="13"/>

</xml_diff>